<commit_message>
Almost done with project.  Added Percolation and PercolationStats.  Need to solve BackWash though.
</commit_message>
<xml_diff>
--- a/algo1/Book1.xlsx
+++ b/algo1/Book1.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="19464"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="19464" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>row</t>
   </si>
@@ -42,6 +43,57 @@
   </si>
   <si>
     <t>Size</t>
+  </si>
+  <si>
+    <t>Site 0</t>
+  </si>
+  <si>
+    <t>Site 1</t>
+  </si>
+  <si>
+    <t>Site 2</t>
+  </si>
+  <si>
+    <t>Site 3</t>
+  </si>
+  <si>
+    <t>Site 4</t>
+  </si>
+  <si>
+    <t>Site 5</t>
+  </si>
+  <si>
+    <t>Site 6</t>
+  </si>
+  <si>
+    <t>Site 7</t>
+  </si>
+  <si>
+    <t>Site 8</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>Open Sites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Open Site 1,2
+- mark site as open
+- Execute Union Find Operations to link to it's neighbors
+- Using my copy of neighbors that are open, link everyone together
+</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Open site 2,2
+- Mark site as open
+- </t>
   </si>
 </sst>
 </file>
@@ -103,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -111,6 +163,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -782,4 +846,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>2</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="5">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>